<commit_message>
include Vera's code, latest data management operations and renv snapshot for reproducibility
</commit_message>
<xml_diff>
--- a/data/data-raw/Table of compounds_030622.xlsx
+++ b/data/data-raw/Table of compounds_030622.xlsx
@@ -3,13 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="14" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C2299E5-814C-491F-98C0-63B5A0166197}"/>
+  <xr:revisionPtr revIDLastSave="221" documentId="11_C9C3E2DFE6E5ECF5CE906EFDC2549BB3DEDA2518" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D17792E5-65CF-4AEA-B598-B2EB92848439}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Experimental Design" sheetId="2" r:id="rId1"/>
     <sheet name="Drugs Mapping" sheetId="3" r:id="rId2"/>
+    <sheet name="Batch Mapping" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
   <extLst>
@@ -20,8 +21,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={5CC803C2-7ABE-4A92-82B1-72B88A9AD957}</author>
+  </authors>
+  <commentList>
+    <comment ref="C16" authorId="0" shapeId="0" xr:uid="{5CC803C2-7ABE-4A92-82B1-72B88A9AD957}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Removed all "Control - time zero" expressions, as I could not match any of them</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="891" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="392">
   <si>
     <t>Samples</t>
   </si>
@@ -149,9 +168,6 @@
     <t>RAF265</t>
   </si>
   <si>
-    <t>Sotorasib (AMG-510)</t>
-  </si>
-  <si>
     <t>35 uM</t>
   </si>
   <si>
@@ -1047,13 +1063,212 @@
   </si>
   <si>
     <t>Mefloq</t>
+  </si>
+  <si>
+    <t>exp010821</t>
+  </si>
+  <si>
+    <t>exp040821</t>
+  </si>
+  <si>
+    <t>exp300821</t>
+  </si>
+  <si>
+    <t>exp200921</t>
+  </si>
+  <si>
+    <t>exp181021</t>
+  </si>
+  <si>
+    <t>exp151121</t>
+  </si>
+  <si>
+    <t>exp070222</t>
+  </si>
+  <si>
+    <t>exp220322</t>
+  </si>
+  <si>
+    <t>Batch_ID</t>
+  </si>
+  <si>
+    <t>exp130921_in vivo</t>
+  </si>
+  <si>
+    <t>exp211221</t>
+  </si>
+  <si>
+    <t>exp200921_dose response osim</t>
+  </si>
+  <si>
+    <t>Excluded experiences</t>
+  </si>
+  <si>
+    <t>exp300821_cor</t>
+  </si>
+  <si>
+    <t>exp281022_time course</t>
+  </si>
+  <si>
+    <t>exp211221cor</t>
+  </si>
+  <si>
+    <t>exp130921_1</t>
+  </si>
+  <si>
+    <t>exp130921</t>
+  </si>
+  <si>
+    <t>exp130921 is complete (more barcode Ids, and more colnames avalaible)</t>
+  </si>
+  <si>
+    <t>Same datasets, except that exp300821 keeps empty columns for no reason.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> exp281022</t>
+  </si>
+  <si>
+    <t>exp281022_mod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On shared probe Ids, the 4 controls have the same expression between both experiences. However, some are present in dose response, some only in the other experiment. </t>
+  </si>
+  <si>
+    <t>In vivo not considered? Currently marked as excluded in Vera's code.</t>
+  </si>
+  <si>
+    <t>Both experiences are recent. Have to check the control samples</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> Exp281022 is the most complete (same barcode Ids, but more samples sequenced). </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Both experiences are recent</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Have to check the control samples</t>
+    </r>
+  </si>
+  <si>
+    <t>ctl</t>
+  </si>
+  <si>
+    <t>protac</t>
+  </si>
+  <si>
+    <t>Ctrl</t>
+  </si>
+  <si>
+    <t>Cetuximab</t>
+  </si>
+  <si>
+    <t>cetux</t>
+  </si>
+  <si>
+    <t>Filename</t>
+  </si>
+  <si>
+    <t>exp130921_vivo</t>
+  </si>
+  <si>
+    <t>exp200921_dose</t>
+  </si>
+  <si>
+    <t>exp281022_time</t>
+  </si>
+  <si>
+    <t>exp271221</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exp211221cor is the most complete (same colnames, but more sampled barcode IDs). </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Dates do not match</t>
+    </r>
+  </si>
+  <si>
+    <t>y-27632 dihydrochloride</t>
+  </si>
+  <si>
+    <t>Sotora</t>
+  </si>
+  <si>
+    <t>BGJ398</t>
+  </si>
+  <si>
+    <t>Crizot</t>
+  </si>
+  <si>
+    <t>TAE684</t>
+  </si>
+  <si>
+    <t>Suniti</t>
+  </si>
+  <si>
+    <t>Plurip</t>
+  </si>
+  <si>
+    <t>Trimet</t>
+  </si>
+  <si>
+    <t>NAcety</t>
+  </si>
+  <si>
+    <t>Nutlin</t>
+  </si>
+  <si>
+    <t>Ibudil</t>
+  </si>
+  <si>
+    <t>NaButy</t>
+  </si>
+  <si>
+    <t>Tricho</t>
+  </si>
+  <si>
+    <t>MG132z</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1112,6 +1327,44 @@
       <color rgb="FF000000"/>
       <name val="Courier New"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="9"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="7"/>
+      <color theme="5"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <color rgb="FF000000"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1936,7 +2189,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="350">
+  <cellXfs count="366">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -2350,6 +2603,48 @@
     <xf numFmtId="0" fontId="7" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2633,7 +2928,51 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="6">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <name val="Courier New"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="7"/>
+        <color rgb="FF000000"/>
+        <name val="Courier New"/>
+        <family val="3"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2696,11 +3035,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A9CE039-12FB-4A5F-A68F-777D338F2EE2}" name="Table1" displayName="Table1" ref="A1:B77" totalsRowShown="0">
-  <autoFilter ref="A1:B77" xr:uid="{1A9CE039-12FB-4A5F-A68F-777D338F2EE2}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1A9CE039-12FB-4A5F-A68F-777D338F2EE2}" name="Table1" displayName="Table1" ref="A1:B97" totalsRowShown="0">
+  <autoFilter ref="A1:B97" xr:uid="{1A9CE039-12FB-4A5F-A68F-777D338F2EE2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B81">
+    <sortCondition ref="A1:A81"/>
+  </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{C833621C-1E47-4C45-8F7B-9F496D081E23}" name="Samples" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{0569DB07-56D4-46A1-8998-DAE8B18F7DD3}" name="Samples_ID" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{C833621C-1E47-4C45-8F7B-9F496D081E23}" name="Samples" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{0569DB07-56D4-46A1-8998-DAE8B18F7DD3}" name="Samples_ID" dataDxfId="4"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C2EBFDB7-7C0A-4BD5-A04E-4602FDC4A7D2}" name="Table2" displayName="Table2" ref="A1:D15" totalsRowShown="0">
+  <autoFilter ref="A1:D15" xr:uid="{C2EBFDB7-7C0A-4BD5-A04E-4602FDC4A7D2}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:C13">
+    <sortCondition ref="B1:B13"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="4" xr3:uid="{2F51DC44-A16D-4C87-B8E4-4754ADD10661}" name="Batch_ID" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{E8A761DC-B001-4CC8-AFA4-5FBC1C1B9527}" name="Filename" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{1D0F9CB7-8150-4F4B-8898-BFF850A5FB44}" name="Excluded experiences" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{A50C6C58-7396-4D5C-8AE7-361FA1E3F9C2}" name="Comments" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2967,12 +3325,20 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="C16" dT="2025-02-23T21:57:24.45" personId="{00000000-0000-0000-0000-000000000000}" id="{5CC803C2-7ABE-4A92-82B1-72B88A9AD957}">
+    <text>Removed all "Control - time zero" expressions, as I could not match any of them</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M254"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3008,17 +3374,17 @@
         <v>2</v>
       </c>
       <c r="H1" s="33" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="277" t="s">
-        <v>144</v>
-      </c>
-      <c r="B2" s="291" t="s">
+      <c r="A2" s="293" t="s">
         <v>143</v>
       </c>
-      <c r="C2" s="295"/>
+      <c r="B2" s="307" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="311"/>
       <c r="D2" s="4">
         <v>2</v>
       </c>
@@ -3032,9 +3398,9 @@
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A3" s="278"/>
-      <c r="B3" s="346"/>
-      <c r="C3" s="296"/>
+      <c r="A3" s="294"/>
+      <c r="B3" s="362"/>
+      <c r="C3" s="312"/>
       <c r="D3" s="4">
         <v>2</v>
       </c>
@@ -3048,9 +3414,9 @@
       <c r="H3" s="8"/>
     </row>
     <row r="4" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A4" s="278"/>
-      <c r="B4" s="346"/>
-      <c r="C4" s="296"/>
+      <c r="A4" s="294"/>
+      <c r="B4" s="362"/>
+      <c r="C4" s="312"/>
       <c r="D4" s="5" t="s">
         <v>10</v>
       </c>
@@ -3064,9 +3430,9 @@
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="278"/>
-      <c r="B5" s="346"/>
-      <c r="C5" s="296"/>
+      <c r="A5" s="294"/>
+      <c r="B5" s="362"/>
+      <c r="C5" s="312"/>
       <c r="D5" s="5" t="s">
         <v>10</v>
       </c>
@@ -3080,9 +3446,9 @@
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A6" s="278"/>
-      <c r="B6" s="346"/>
-      <c r="C6" s="296"/>
+      <c r="A6" s="294"/>
+      <c r="B6" s="362"/>
+      <c r="C6" s="312"/>
       <c r="D6" s="5" t="s">
         <v>13</v>
       </c>
@@ -3096,9 +3462,9 @@
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="278"/>
-      <c r="B7" s="346"/>
-      <c r="C7" s="296"/>
+      <c r="A7" s="294"/>
+      <c r="B7" s="362"/>
+      <c r="C7" s="312"/>
       <c r="D7" s="5" t="s">
         <v>13</v>
       </c>
@@ -3112,102 +3478,102 @@
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="278"/>
-      <c r="B8" s="346"/>
-      <c r="C8" s="296"/>
-      <c r="D8" s="264" t="s">
+      <c r="A8" s="294"/>
+      <c r="B8" s="362"/>
+      <c r="C8" s="312"/>
+      <c r="D8" s="280" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264" t="s">
+      <c r="E8" s="280"/>
+      <c r="F8" s="280" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="264" t="s">
-        <v>153</v>
-      </c>
-      <c r="H8" s="266" t="s">
-        <v>91</v>
+      <c r="G8" s="280" t="s">
+        <v>152</v>
+      </c>
+      <c r="H8" s="282" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="278"/>
-      <c r="B9" s="346"/>
-      <c r="C9" s="296"/>
-      <c r="D9" s="265"/>
-      <c r="E9" s="265"/>
-      <c r="F9" s="265"/>
-      <c r="G9" s="265"/>
-      <c r="H9" s="267"/>
+      <c r="A9" s="294"/>
+      <c r="B9" s="362"/>
+      <c r="C9" s="312"/>
+      <c r="D9" s="281"/>
+      <c r="E9" s="281"/>
+      <c r="F9" s="281"/>
+      <c r="G9" s="281"/>
+      <c r="H9" s="283"/>
     </row>
     <row r="10" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="278"/>
-      <c r="B10" s="346"/>
-      <c r="C10" s="297"/>
-      <c r="D10" s="270" t="s">
+      <c r="A10" s="294"/>
+      <c r="B10" s="362"/>
+      <c r="C10" s="313"/>
+      <c r="D10" s="286" t="s">
         <v>13</v>
       </c>
-      <c r="E10" s="272"/>
-      <c r="F10" s="270" t="s">
+      <c r="E10" s="288"/>
+      <c r="F10" s="286" t="s">
         <v>16</v>
       </c>
-      <c r="G10" s="270" t="s">
-        <v>153</v>
-      </c>
-      <c r="H10" s="275" t="s">
-        <v>91</v>
+      <c r="G10" s="286" t="s">
+        <v>152</v>
+      </c>
+      <c r="H10" s="291" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="278"/>
-      <c r="B11" s="346"/>
-      <c r="C11" s="297"/>
-      <c r="D11" s="271"/>
-      <c r="E11" s="273"/>
-      <c r="F11" s="274"/>
-      <c r="G11" s="274"/>
-      <c r="H11" s="276"/>
+      <c r="A11" s="294"/>
+      <c r="B11" s="362"/>
+      <c r="C11" s="313"/>
+      <c r="D11" s="287"/>
+      <c r="E11" s="289"/>
+      <c r="F11" s="290"/>
+      <c r="G11" s="290"/>
+      <c r="H11" s="292"/>
       <c r="I11" s="205"/>
     </row>
     <row r="12" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="278"/>
-      <c r="B12" s="346"/>
-      <c r="C12" s="297"/>
+      <c r="A12" s="294"/>
+      <c r="B12" s="362"/>
+      <c r="C12" s="313"/>
       <c r="D12" s="204" t="s">
         <v>13</v>
       </c>
       <c r="E12" s="208"/>
       <c r="F12" s="141" t="s">
+        <v>198</v>
+      </c>
+      <c r="G12" s="141" t="s">
         <v>199</v>
-      </c>
-      <c r="G12" s="141" t="s">
-        <v>200</v>
       </c>
       <c r="H12" s="206"/>
       <c r="I12" s="205"/>
     </row>
     <row r="13" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="278"/>
-      <c r="B13" s="347"/>
-      <c r="C13" s="298"/>
+      <c r="A13" s="294"/>
+      <c r="B13" s="363"/>
+      <c r="C13" s="314"/>
       <c r="D13" s="203" t="s">
         <v>13</v>
       </c>
       <c r="E13" s="209"/>
       <c r="F13" s="203" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G13" s="203" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H13" s="207"/>
       <c r="I13" s="205"/>
     </row>
     <row r="14" spans="1:9" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="278"/>
-      <c r="B14" s="291" t="s">
+      <c r="A14" s="294"/>
+      <c r="B14" s="307" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="295"/>
+      <c r="C14" s="311"/>
       <c r="D14" s="4" t="s">
         <v>18</v>
       </c>
@@ -3221,9 +3587,9 @@
       <c r="H14" s="7"/>
     </row>
     <row r="15" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="278"/>
-      <c r="B15" s="292"/>
-      <c r="C15" s="322"/>
+      <c r="A15" s="294"/>
+      <c r="B15" s="308"/>
+      <c r="C15" s="338"/>
       <c r="D15" s="5" t="s">
         <v>18</v>
       </c>
@@ -3237,9 +3603,9 @@
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:9" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="278"/>
-      <c r="B16" s="292"/>
-      <c r="C16" s="322"/>
+      <c r="A16" s="294"/>
+      <c r="B16" s="308"/>
+      <c r="C16" s="338"/>
       <c r="D16" s="5" t="s">
         <v>18</v>
       </c>
@@ -3253,9 +3619,9 @@
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="278"/>
-      <c r="B17" s="292"/>
-      <c r="C17" s="322"/>
+      <c r="A17" s="294"/>
+      <c r="B17" s="308"/>
+      <c r="C17" s="338"/>
       <c r="D17" s="5" t="s">
         <v>18</v>
       </c>
@@ -3269,9 +3635,9 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="278"/>
-      <c r="B18" s="292"/>
-      <c r="C18" s="322"/>
+      <c r="A18" s="294"/>
+      <c r="B18" s="308"/>
+      <c r="C18" s="338"/>
       <c r="D18" s="5" t="s">
         <v>18</v>
       </c>
@@ -3285,9 +3651,9 @@
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="278"/>
-      <c r="B19" s="292"/>
-      <c r="C19" s="322"/>
+      <c r="A19" s="294"/>
+      <c r="B19" s="308"/>
+      <c r="C19" s="338"/>
       <c r="D19" s="5" t="s">
         <v>18</v>
       </c>
@@ -3301,9 +3667,9 @@
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="278"/>
-      <c r="B20" s="292"/>
-      <c r="C20" s="323"/>
+      <c r="A20" s="294"/>
+      <c r="B20" s="308"/>
+      <c r="C20" s="339"/>
       <c r="D20" s="12" t="s">
         <v>18</v>
       </c>
@@ -3317,69 +3683,69 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="278"/>
-      <c r="B21" s="292"/>
-      <c r="C21" s="323"/>
-      <c r="D21" s="255" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="255"/>
-      <c r="F21" s="255" t="s">
+      <c r="A21" s="294"/>
+      <c r="B21" s="308"/>
+      <c r="C21" s="339"/>
+      <c r="D21" s="271" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="271"/>
+      <c r="F21" s="271" t="s">
         <v>16</v>
       </c>
-      <c r="G21" s="255" t="s">
-        <v>153</v>
-      </c>
-      <c r="H21" s="257" t="s">
-        <v>91</v>
+      <c r="G21" s="271" t="s">
+        <v>152</v>
+      </c>
+      <c r="H21" s="273" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A22" s="278"/>
-      <c r="B22" s="292"/>
-      <c r="C22" s="323"/>
-      <c r="D22" s="256"/>
-      <c r="E22" s="256"/>
-      <c r="F22" s="256"/>
-      <c r="G22" s="256"/>
-      <c r="H22" s="258"/>
+      <c r="A22" s="294"/>
+      <c r="B22" s="308"/>
+      <c r="C22" s="339"/>
+      <c r="D22" s="272"/>
+      <c r="E22" s="272"/>
+      <c r="F22" s="272"/>
+      <c r="G22" s="272"/>
+      <c r="H22" s="274"/>
     </row>
     <row r="23" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="278"/>
-      <c r="B23" s="292"/>
-      <c r="C23" s="323"/>
+      <c r="A23" s="294"/>
+      <c r="B23" s="308"/>
+      <c r="C23" s="339"/>
       <c r="D23" s="24" t="s">
         <v>18</v>
       </c>
       <c r="E23" s="21"/>
       <c r="F23" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="G23" s="21" t="s">
         <v>199</v>
       </c>
-      <c r="G23" s="21" t="s">
-        <v>200</v>
-      </c>
       <c r="H23" s="143"/>
     </row>
     <row r="24" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="278"/>
-      <c r="B24" s="292"/>
-      <c r="C24" s="323"/>
+      <c r="A24" s="294"/>
+      <c r="B24" s="308"/>
+      <c r="C24" s="339"/>
       <c r="D24" s="142" t="s">
         <v>18</v>
       </c>
       <c r="E24" s="142"/>
       <c r="F24" s="142" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G24" s="142" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H24" s="144"/>
     </row>
     <row r="25" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="279"/>
-      <c r="B25" s="292"/>
-      <c r="C25" s="324"/>
+      <c r="A25" s="295"/>
+      <c r="B25" s="308"/>
+      <c r="C25" s="340"/>
       <c r="D25" s="120" t="s">
         <v>19</v>
       </c>
@@ -3395,13 +3761,13 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="325" t="s">
+      <c r="A26" s="341" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="293" t="s">
-        <v>146</v>
-      </c>
-      <c r="C26" s="301" t="s">
+      <c r="B26" s="309" t="s">
+        <v>145</v>
+      </c>
+      <c r="C26" s="317" t="s">
         <v>25</v>
       </c>
       <c r="D26" s="122" t="s">
@@ -3421,9 +3787,9 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="326"/>
-      <c r="B27" s="331"/>
-      <c r="C27" s="302"/>
+      <c r="A27" s="342"/>
+      <c r="B27" s="347"/>
+      <c r="C27" s="318"/>
       <c r="D27" s="125" t="s">
         <v>18</v>
       </c>
@@ -3439,9 +3805,9 @@
       <c r="H27" s="127"/>
     </row>
     <row r="28" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="326"/>
-      <c r="B28" s="331"/>
-      <c r="C28" s="302"/>
+      <c r="A28" s="342"/>
+      <c r="B28" s="347"/>
+      <c r="C28" s="318"/>
       <c r="D28" s="128" t="s">
         <v>18</v>
       </c>
@@ -3457,9 +3823,9 @@
       <c r="H28" s="129"/>
     </row>
     <row r="29" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A29" s="326"/>
-      <c r="B29" s="331"/>
-      <c r="C29" s="302"/>
+      <c r="A29" s="342"/>
+      <c r="B29" s="347"/>
+      <c r="C29" s="318"/>
       <c r="D29" s="128" t="s">
         <v>18</v>
       </c>
@@ -3475,9 +3841,9 @@
       <c r="H29" s="129"/>
     </row>
     <row r="30" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="326"/>
-      <c r="B30" s="331"/>
-      <c r="C30" s="302"/>
+      <c r="A30" s="342"/>
+      <c r="B30" s="347"/>
+      <c r="C30" s="318"/>
       <c r="D30" s="128" t="s">
         <v>18</v>
       </c>
@@ -3493,9 +3859,9 @@
       <c r="H30" s="129"/>
     </row>
     <row r="31" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="326"/>
-      <c r="B31" s="331"/>
-      <c r="C31" s="302"/>
+      <c r="A31" s="342"/>
+      <c r="B31" s="347"/>
+      <c r="C31" s="318"/>
       <c r="D31" s="128" t="s">
         <v>18</v>
       </c>
@@ -3511,9 +3877,9 @@
       <c r="H31" s="129"/>
     </row>
     <row r="32" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="326"/>
-      <c r="B32" s="331"/>
-      <c r="C32" s="302"/>
+      <c r="A32" s="342"/>
+      <c r="B32" s="347"/>
+      <c r="C32" s="318"/>
       <c r="D32" s="128" t="s">
         <v>18</v>
       </c>
@@ -3529,9 +3895,9 @@
       <c r="H32" s="129"/>
     </row>
     <row r="33" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A33" s="326"/>
-      <c r="B33" s="331"/>
-      <c r="C33" s="303"/>
+      <c r="A33" s="342"/>
+      <c r="B33" s="347"/>
+      <c r="C33" s="319"/>
       <c r="D33" s="166" t="s">
         <v>18</v>
       </c>
@@ -3547,8 +3913,8 @@
       <c r="H33" s="168"/>
     </row>
     <row r="34" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="326"/>
-      <c r="B34" s="331"/>
+      <c r="A34" s="342"/>
+      <c r="B34" s="347"/>
       <c r="C34" s="138" t="s">
         <v>35</v>
       </c>
@@ -3565,75 +3931,75 @@
         <v>36</v>
       </c>
       <c r="H34" s="193" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="326"/>
-      <c r="B35" s="331"/>
+      <c r="A35" s="342"/>
+      <c r="B35" s="347"/>
       <c r="C35" s="188" t="s">
+        <v>213</v>
+      </c>
+      <c r="D35" s="190" t="s">
+        <v>18</v>
+      </c>
+      <c r="E35" s="190" t="s">
+        <v>216</v>
+      </c>
+      <c r="F35" s="132" t="s">
+        <v>198</v>
+      </c>
+      <c r="G35" s="132" t="s">
+        <v>199</v>
+      </c>
+      <c r="H35" s="194"/>
+    </row>
+    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A36" s="342"/>
+      <c r="B36" s="347"/>
+      <c r="C36" s="188" t="s">
         <v>214</v>
       </c>
-      <c r="D35" s="190" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="190" t="s">
-        <v>217</v>
-      </c>
-      <c r="F35" s="132" t="s">
+      <c r="D36" s="190" t="s">
+        <v>18</v>
+      </c>
+      <c r="E36" s="192" t="s">
+        <v>216</v>
+      </c>
+      <c r="F36" s="136" t="s">
+        <v>198</v>
+      </c>
+      <c r="G36" s="189" t="s">
         <v>199</v>
       </c>
-      <c r="G35" s="132" t="s">
-        <v>200</v>
-      </c>
-      <c r="H35" s="194"/>
-    </row>
-    <row r="36" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A36" s="326"/>
-      <c r="B36" s="331"/>
-      <c r="C36" s="188" t="s">
+      <c r="H36" s="194"/>
+    </row>
+    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A37" s="342"/>
+      <c r="B37" s="310"/>
+      <c r="C37" s="165" t="s">
         <v>215</v>
       </c>
-      <c r="D36" s="190" t="s">
-        <v>18</v>
-      </c>
-      <c r="E36" s="192" t="s">
-        <v>217</v>
-      </c>
-      <c r="F36" s="136" t="s">
+      <c r="D37" s="191" t="s">
+        <v>18</v>
+      </c>
+      <c r="E37" s="164" t="s">
+        <v>216</v>
+      </c>
+      <c r="F37" s="190" t="s">
+        <v>198</v>
+      </c>
+      <c r="G37" s="190" t="s">
         <v>199</v>
       </c>
-      <c r="G36" s="189" t="s">
-        <v>200</v>
-      </c>
-      <c r="H36" s="194"/>
-    </row>
-    <row r="37" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A37" s="326"/>
-      <c r="B37" s="294"/>
-      <c r="C37" s="165" t="s">
-        <v>216</v>
-      </c>
-      <c r="D37" s="191" t="s">
-        <v>18</v>
-      </c>
-      <c r="E37" s="164" t="s">
-        <v>217</v>
-      </c>
-      <c r="F37" s="190" t="s">
-        <v>199</v>
-      </c>
-      <c r="G37" s="190" t="s">
-        <v>200</v>
-      </c>
       <c r="H37" s="195"/>
     </row>
     <row r="38" spans="1:13" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="326"/>
-      <c r="B38" s="293" t="s">
-        <v>147</v>
-      </c>
-      <c r="C38" s="302" t="s">
+      <c r="A38" s="342"/>
+      <c r="B38" s="309" t="s">
+        <v>146</v>
+      </c>
+      <c r="C38" s="318" t="s">
         <v>32</v>
       </c>
       <c r="D38" s="125" t="s">
@@ -3651,9 +4017,9 @@
       <c r="H38" s="127"/>
     </row>
     <row r="39" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A39" s="326"/>
-      <c r="B39" s="294"/>
-      <c r="C39" s="302"/>
+      <c r="A39" s="342"/>
+      <c r="B39" s="310"/>
+      <c r="C39" s="318"/>
       <c r="D39" s="132" t="s">
         <v>18</v>
       </c>
@@ -3669,12 +4035,12 @@
       <c r="H39" s="135"/>
     </row>
     <row r="40" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="327"/>
+      <c r="A40" s="343"/>
       <c r="B40" s="170" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C40" s="169" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D40" s="136" t="s">
         <v>18</v>
@@ -3697,17 +4063,17 @@
     </row>
     <row r="41" spans="1:13" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="28" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B41" s="108"/>
       <c r="C41" s="26" t="s">
+        <v>378</v>
+      </c>
+      <c r="D41" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E41" s="26" t="s">
         <v>42</v>
-      </c>
-      <c r="D41" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E41" s="26" t="s">
-        <v>43</v>
       </c>
       <c r="F41" s="26" t="s">
         <v>16</v>
@@ -3716,15 +4082,15 @@
         <v>36</v>
       </c>
       <c r="H41" s="199" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A42" s="332" t="s">
+      <c r="A42" s="348" t="s">
         <v>38</v>
       </c>
       <c r="B42" s="174"/>
-      <c r="C42" s="348" t="s">
+      <c r="C42" s="364" t="s">
         <v>37</v>
       </c>
       <c r="D42" s="63" t="s">
@@ -3742,9 +4108,9 @@
       <c r="H42" s="197"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="333"/>
+      <c r="A43" s="349"/>
       <c r="B43" s="174"/>
-      <c r="C43" s="349"/>
+      <c r="C43" s="365"/>
       <c r="D43" s="66" t="s">
         <v>18</v>
       </c>
@@ -3760,9 +4126,9 @@
       <c r="H43" s="198"/>
     </row>
     <row r="44" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="333"/>
+      <c r="A44" s="349"/>
       <c r="B44" s="174"/>
-      <c r="C44" s="348" t="s">
+      <c r="C44" s="364" t="s">
         <v>39</v>
       </c>
       <c r="D44" s="63" t="s">
@@ -3780,9 +4146,9 @@
       <c r="H44" s="197"/>
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A45" s="333"/>
+      <c r="A45" s="349"/>
       <c r="B45" s="174"/>
-      <c r="C45" s="349"/>
+      <c r="C45" s="365"/>
       <c r="D45" s="66" t="s">
         <v>18</v>
       </c>
@@ -3798,7 +4164,7 @@
       <c r="H45" s="198"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A46" s="333"/>
+      <c r="A46" s="349"/>
       <c r="B46" s="211"/>
       <c r="C46" s="212" t="s">
         <v>41</v>
@@ -3818,38 +4184,38 @@
       <c r="H46" s="216"/>
     </row>
     <row r="47" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A47" s="334"/>
+      <c r="A47" s="350"/>
       <c r="B47" s="109"/>
       <c r="C47" s="70" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D47" s="69" t="s">
         <v>18</v>
       </c>
       <c r="E47" s="70" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F47" s="69" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G47" s="71" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H47" s="72"/>
     </row>
     <row r="48" spans="1:13" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="278" t="s">
-        <v>47</v>
+      <c r="A48" s="294" t="s">
+        <v>46</v>
       </c>
       <c r="B48" s="110"/>
-      <c r="C48" s="304" t="s">
+      <c r="C48" s="320" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="D48" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="F48" s="210" t="s">
         <v>6</v>
@@ -3860,14 +4226,14 @@
       <c r="H48" s="200"/>
     </row>
     <row r="49" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="278"/>
+      <c r="A49" s="294"/>
       <c r="B49" s="110"/>
-      <c r="C49" s="304"/>
+      <c r="C49" s="320"/>
       <c r="D49" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F49" s="16" t="s">
         <v>20</v>
@@ -3878,14 +4244,14 @@
       <c r="H49" s="8"/>
     </row>
     <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A50" s="278"/>
+      <c r="A50" s="294"/>
       <c r="B50" s="110"/>
-      <c r="C50" s="304"/>
+      <c r="C50" s="320"/>
       <c r="D50" s="12" t="s">
         <v>18</v>
       </c>
       <c r="E50" s="12" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F50" s="23" t="s">
         <v>15</v>
@@ -3896,16 +4262,16 @@
       <c r="H50" s="12"/>
     </row>
     <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="279"/>
+      <c r="A51" s="295"/>
       <c r="B51" s="175"/>
       <c r="C51" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D51" s="42">
         <v>4</v>
       </c>
       <c r="E51" s="36" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F51" s="37" t="s">
         <v>15</v>
@@ -3916,14 +4282,14 @@
       <c r="H51" s="42"/>
     </row>
     <row r="52" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="299" t="s">
-        <v>54</v>
+      <c r="A52" s="315" t="s">
+        <v>53</v>
       </c>
       <c r="B52" s="111" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C52" s="173" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="73" t="s">
         <v>18</v>
@@ -3938,16 +4304,16 @@
         <v>36</v>
       </c>
       <c r="H52" s="73" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="300"/>
+      <c r="A53" s="316"/>
       <c r="B53" s="112" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C53" s="76" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D53" s="75" t="s">
         <v>18</v>
@@ -3962,22 +4328,22 @@
         <v>36</v>
       </c>
       <c r="H53" s="75" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A54" s="29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B54" s="176"/>
       <c r="C54" s="45" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D54" s="43" t="s">
         <v>18</v>
       </c>
       <c r="E54" s="43" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F54" s="44" t="s">
         <v>16</v>
@@ -3986,24 +4352,24 @@
         <v>36</v>
       </c>
       <c r="H54" s="43" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="343" t="s">
-        <v>152</v>
-      </c>
-      <c r="B55" s="338" t="s">
-        <v>149</v>
-      </c>
-      <c r="C55" s="285" t="s">
+      <c r="A55" s="359" t="s">
+        <v>151</v>
+      </c>
+      <c r="B55" s="354" t="s">
+        <v>148</v>
+      </c>
+      <c r="C55" s="301" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E55" s="57" t="s">
         <v>58</v>
-      </c>
-      <c r="D55" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E55" s="57" t="s">
-        <v>59</v>
       </c>
       <c r="F55" s="58" t="s">
         <v>6</v>
@@ -4014,14 +4380,14 @@
       <c r="H55" s="57"/>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="344"/>
-      <c r="B56" s="339"/>
-      <c r="C56" s="286"/>
+      <c r="A56" s="360"/>
+      <c r="B56" s="355"/>
+      <c r="C56" s="302"/>
       <c r="D56" s="46" t="s">
         <v>18</v>
       </c>
       <c r="E56" s="46" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F56" s="47" t="s">
         <v>20</v>
@@ -4032,76 +4398,76 @@
       <c r="H56" s="46"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A57" s="344"/>
-      <c r="B57" s="339"/>
-      <c r="C57" s="287"/>
+      <c r="A57" s="360"/>
+      <c r="B57" s="355"/>
+      <c r="C57" s="303"/>
       <c r="D57" s="59" t="s">
         <v>18</v>
       </c>
       <c r="E57" s="59" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F57" s="60" t="s">
         <v>14</v>
       </c>
       <c r="G57" s="59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H57" s="59"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="344"/>
-      <c r="B58" s="340"/>
+      <c r="A58" s="360"/>
+      <c r="B58" s="356"/>
       <c r="C58" s="239" t="s">
+        <v>227</v>
+      </c>
+      <c r="D58" s="236" t="s">
+        <v>18</v>
+      </c>
+      <c r="E58" s="236" t="s">
+        <v>47</v>
+      </c>
+      <c r="F58" s="236" t="s">
+        <v>230</v>
+      </c>
+      <c r="G58" s="236" t="s">
+        <v>220</v>
+      </c>
+      <c r="H58" s="236"/>
+    </row>
+    <row r="59" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A59" s="360"/>
+      <c r="B59" s="357"/>
+      <c r="C59" s="239" t="s">
         <v>228</v>
       </c>
-      <c r="D58" s="236" t="s">
-        <v>18</v>
-      </c>
-      <c r="E58" s="236" t="s">
-        <v>48</v>
-      </c>
-      <c r="F58" s="236" t="s">
-        <v>231</v>
-      </c>
-      <c r="G58" s="236" t="s">
-        <v>221</v>
-      </c>
-      <c r="H58" s="236"/>
-    </row>
-    <row r="59" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A59" s="344"/>
-      <c r="B59" s="341"/>
-      <c r="C59" s="239" t="s">
+      <c r="D59" s="236" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="236" t="s">
         <v>229</v>
       </c>
-      <c r="D59" s="236" t="s">
-        <v>18</v>
-      </c>
-      <c r="E59" s="236" t="s">
+      <c r="F59" s="236" t="s">
         <v>230</v>
       </c>
-      <c r="F59" s="236" t="s">
-        <v>231</v>
-      </c>
       <c r="G59" s="236" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H59" s="236"/>
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="344"/>
-      <c r="B60" s="338" t="s">
-        <v>150</v>
-      </c>
-      <c r="C60" s="285" t="s">
+      <c r="A60" s="360"/>
+      <c r="B60" s="354" t="s">
+        <v>149</v>
+      </c>
+      <c r="C60" s="301" t="s">
+        <v>61</v>
+      </c>
+      <c r="D60" s="57" t="s">
+        <v>18</v>
+      </c>
+      <c r="E60" s="57" t="s">
         <v>62</v>
-      </c>
-      <c r="D60" s="57" t="s">
-        <v>18</v>
-      </c>
-      <c r="E60" s="57" t="s">
-        <v>63</v>
       </c>
       <c r="F60" s="58" t="s">
         <v>21</v>
@@ -4112,28 +4478,28 @@
       <c r="H60" s="57"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="344"/>
-      <c r="B61" s="339"/>
-      <c r="C61" s="287"/>
+      <c r="A61" s="360"/>
+      <c r="B61" s="355"/>
+      <c r="C61" s="303"/>
       <c r="D61" s="59" t="s">
         <v>18</v>
       </c>
       <c r="E61" s="59" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F61" s="61" t="s">
         <v>14</v>
       </c>
       <c r="G61" s="59" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H61" s="59"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="344"/>
-      <c r="B62" s="339"/>
+      <c r="A62" s="360"/>
+      <c r="B62" s="355"/>
       <c r="C62" s="172" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D62" s="240" t="s">
         <v>18</v>
@@ -4142,68 +4508,68 @@
         <v>31</v>
       </c>
       <c r="F62" s="243" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G62" s="62" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H62" s="62"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A63" s="344"/>
-      <c r="B63" s="342"/>
+      <c r="A63" s="360"/>
+      <c r="B63" s="358"/>
       <c r="C63" s="172" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D63" s="240" t="s">
         <v>18</v>
       </c>
       <c r="E63" s="241" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F63" s="242" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G63" s="241" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H63" s="241"/>
     </row>
     <row r="64" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A64" s="344"/>
+      <c r="A64" s="360"/>
       <c r="B64" s="245" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C64" s="62" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D64" s="171" t="s">
         <v>18</v>
       </c>
       <c r="E64" s="62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F64" s="62" t="s">
         <v>14</v>
       </c>
       <c r="G64" s="62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H64" s="62"/>
     </row>
     <row r="65" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A65" s="344"/>
+      <c r="A65" s="360"/>
       <c r="B65" s="246" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C65" s="177" t="s">
+        <v>100</v>
+      </c>
+      <c r="D65" s="177" t="s">
+        <v>18</v>
+      </c>
+      <c r="E65" s="177" t="s">
         <v>101</v>
-      </c>
-      <c r="D65" s="177" t="s">
-        <v>18</v>
-      </c>
-      <c r="E65" s="177" t="s">
-        <v>102</v>
       </c>
       <c r="F65" s="62" t="s">
         <v>15</v>
@@ -4214,64 +4580,64 @@
       <c r="H65" s="177"/>
     </row>
     <row r="66" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A66" s="344"/>
+      <c r="A66" s="360"/>
       <c r="B66" s="247" t="s">
+        <v>233</v>
+      </c>
+      <c r="C66" s="62" t="s">
         <v>234</v>
       </c>
-      <c r="C66" s="62" t="s">
+      <c r="D66" s="62" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="62" t="s">
+        <v>84</v>
+      </c>
+      <c r="F66" s="242" t="s">
+        <v>198</v>
+      </c>
+      <c r="G66" s="62" t="s">
+        <v>220</v>
+      </c>
+      <c r="H66" s="62"/>
+    </row>
+    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A67" s="361"/>
+      <c r="B67" s="244" t="s">
+        <v>237</v>
+      </c>
+      <c r="C67" s="240" t="s">
         <v>235</v>
       </c>
-      <c r="D66" s="62" t="s">
-        <v>18</v>
-      </c>
-      <c r="E66" s="62" t="s">
-        <v>85</v>
-      </c>
-      <c r="F66" s="242" t="s">
-        <v>199</v>
-      </c>
-      <c r="G66" s="62" t="s">
-        <v>221</v>
-      </c>
-      <c r="H66" s="62"/>
-    </row>
-    <row r="67" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="345"/>
-      <c r="B67" s="244" t="s">
-        <v>238</v>
-      </c>
-      <c r="C67" s="240" t="s">
+      <c r="D67" s="241" t="s">
+        <v>18</v>
+      </c>
+      <c r="E67" s="241" t="s">
         <v>236</v>
       </c>
-      <c r="D67" s="241" t="s">
-        <v>18</v>
-      </c>
-      <c r="E67" s="241" t="s">
-        <v>237</v>
-      </c>
       <c r="F67" s="242" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G67" s="241" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H67" s="241"/>
     </row>
     <row r="68" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="277" t="s">
-        <v>154</v>
+      <c r="A68" s="293" t="s">
+        <v>153</v>
       </c>
       <c r="B68" s="238" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C68" s="237" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D68" s="234" t="s">
         <v>18</v>
       </c>
       <c r="E68" s="234" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="F68" s="235" t="s">
         <v>8</v>
@@ -4282,12 +4648,12 @@
       <c r="H68" s="234"/>
     </row>
     <row r="69" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A69" s="278"/>
-      <c r="B69" s="288" t="s">
-        <v>196</v>
+      <c r="A69" s="294"/>
+      <c r="B69" s="304" t="s">
+        <v>195</v>
       </c>
       <c r="C69" s="42" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D69" s="42" t="s">
         <v>18</v>
@@ -4304,103 +4670,103 @@
       <c r="H69" s="42"/>
     </row>
     <row r="70" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A70" s="278"/>
-      <c r="B70" s="289"/>
+      <c r="A70" s="294"/>
+      <c r="B70" s="305"/>
       <c r="C70" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="D70" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E70" s="42" t="s">
         <v>68</v>
-      </c>
-      <c r="D70" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E70" s="42" t="s">
-        <v>69</v>
       </c>
       <c r="F70" s="37" t="s">
         <v>14</v>
       </c>
       <c r="G70" s="42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H70" s="42"/>
     </row>
     <row r="71" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A71" s="278"/>
-      <c r="B71" s="289"/>
+      <c r="A71" s="294"/>
+      <c r="B71" s="305"/>
       <c r="C71" s="42" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D71" s="42" t="s">
         <v>18</v>
       </c>
       <c r="E71" s="42" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F71" s="37" t="s">
         <v>16</v>
       </c>
       <c r="G71" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H71" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A72" s="278"/>
-      <c r="B72" s="290"/>
+      <c r="A72" s="294"/>
+      <c r="B72" s="306"/>
       <c r="C72" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="D72" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E72" s="42" t="s">
         <v>73</v>
-      </c>
-      <c r="D72" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E72" s="42" t="s">
-        <v>74</v>
       </c>
       <c r="F72" s="37" t="s">
         <v>16</v>
       </c>
       <c r="G72" s="42" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H72" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A73" s="279"/>
+      <c r="A73" s="295"/>
       <c r="B73" s="224" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C73" s="22" t="s">
+        <v>69</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="22" t="s">
         <v>70</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E73" s="22" t="s">
-        <v>71</v>
       </c>
       <c r="F73" s="15" t="s">
         <v>14</v>
       </c>
       <c r="G73" s="22" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H73" s="22"/>
     </row>
     <row r="74" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A74" s="314" t="s">
-        <v>160</v>
-      </c>
-      <c r="B74" s="312" t="s">
-        <v>155</v>
-      </c>
-      <c r="C74" s="310" t="s">
+      <c r="A74" s="330" t="s">
+        <v>159</v>
+      </c>
+      <c r="B74" s="328" t="s">
+        <v>154</v>
+      </c>
+      <c r="C74" s="326" t="s">
+        <v>74</v>
+      </c>
+      <c r="D74" s="78" t="s">
         <v>75</v>
-      </c>
-      <c r="D74" s="78" t="s">
-        <v>76</v>
       </c>
       <c r="E74" s="78" t="s">
         <v>31</v>
@@ -4412,18 +4778,18 @@
         <v>9</v>
       </c>
       <c r="H74" s="78" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A75" s="315"/>
-      <c r="B75" s="313"/>
-      <c r="C75" s="311"/>
+      <c r="A75" s="331"/>
+      <c r="B75" s="329"/>
+      <c r="C75" s="327"/>
       <c r="D75" s="80" t="s">
         <v>18</v>
       </c>
       <c r="E75" s="80" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F75" s="81" t="s">
         <v>15</v>
@@ -4434,34 +4800,34 @@
       <c r="H75" s="82"/>
     </row>
     <row r="76" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A76" s="315"/>
+      <c r="A76" s="331"/>
       <c r="B76" s="222" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C76" s="83" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D76" s="83" t="s">
         <v>18</v>
       </c>
       <c r="E76" s="83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F76" s="84" t="s">
         <v>14</v>
       </c>
       <c r="G76" s="83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H76" s="83"/>
     </row>
     <row r="77" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A77" s="315"/>
+      <c r="A77" s="331"/>
       <c r="B77" s="223" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C77" s="83" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D77" s="83" t="s">
         <v>18</v>
@@ -4473,17 +4839,17 @@
         <v>14</v>
       </c>
       <c r="G77" s="83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H77" s="83"/>
     </row>
     <row r="78" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A78" s="315"/>
+      <c r="A78" s="331"/>
       <c r="B78" s="223" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C78" s="83" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D78" s="83" t="s">
         <v>18</v>
@@ -4495,23 +4861,23 @@
         <v>14</v>
       </c>
       <c r="G78" s="83" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H78" s="83"/>
     </row>
     <row r="79" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A79" s="316"/>
+      <c r="A79" s="332"/>
       <c r="B79" s="223" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C79" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="D79" s="85" t="s">
+        <v>18</v>
+      </c>
+      <c r="E79" s="85" t="s">
         <v>81</v>
-      </c>
-      <c r="D79" s="85" t="s">
-        <v>18</v>
-      </c>
-      <c r="E79" s="85" t="s">
-        <v>82</v>
       </c>
       <c r="F79" s="86" t="s">
         <v>16</v>
@@ -4520,24 +4886,24 @@
         <v>36</v>
       </c>
       <c r="H79" s="85" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A80" s="277" t="s">
+      <c r="A80" s="293" t="s">
+        <v>160</v>
+      </c>
+      <c r="B80" s="220" t="s">
         <v>161</v>
       </c>
-      <c r="B80" s="220" t="s">
-        <v>162</v>
-      </c>
       <c r="C80" s="36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D80" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E80" s="42" t="s">
         <v>84</v>
-      </c>
-      <c r="D80" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E80" s="42" t="s">
-        <v>85</v>
       </c>
       <c r="F80" s="37" t="s">
         <v>21</v>
@@ -4548,12 +4914,12 @@
       <c r="H80" s="42"/>
     </row>
     <row r="81" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A81" s="279"/>
+      <c r="A81" s="295"/>
       <c r="B81" s="221" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C81" s="20" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D81" s="17" t="s">
         <v>18</v>
@@ -4568,18 +4934,18 @@
         <v>36</v>
       </c>
       <c r="H81" s="17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A82" s="319" t="s">
-        <v>166</v>
-      </c>
-      <c r="B82" s="317" t="s">
-        <v>164</v>
+      <c r="A82" s="335" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="333" t="s">
+        <v>163</v>
       </c>
       <c r="C82" s="49" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D82" s="48" t="s">
         <v>18</v>
@@ -4596,34 +4962,34 @@
       <c r="H82" s="48"/>
     </row>
     <row r="83" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A83" s="320"/>
-      <c r="B83" s="318"/>
+      <c r="A83" s="336"/>
+      <c r="B83" s="334"/>
       <c r="C83" s="51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D83" s="50" t="s">
         <v>18</v>
       </c>
       <c r="E83" s="50" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F83" s="52" t="s">
         <v>15</v>
       </c>
       <c r="G83" s="50" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H83" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A84" s="321"/>
+      <c r="A84" s="337"/>
       <c r="B84" s="114" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C84" s="54" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D84" s="53" t="s">
         <v>18</v>
@@ -4640,12 +5006,12 @@
       <c r="H84" s="53"/>
     </row>
     <row r="85" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A85" s="277" t="s">
-        <v>167</v>
+      <c r="A85" s="293" t="s">
+        <v>166</v>
       </c>
       <c r="B85" s="179"/>
-      <c r="C85" s="268" t="s">
-        <v>92</v>
+      <c r="C85" s="284" t="s">
+        <v>91</v>
       </c>
       <c r="D85" s="39" t="s">
         <v>18</v>
@@ -4662,9 +5028,9 @@
       <c r="H85" s="38"/>
     </row>
     <row r="86" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A86" s="278"/>
+      <c r="A86" s="294"/>
       <c r="B86" s="180"/>
-      <c r="C86" s="269"/>
+      <c r="C86" s="285"/>
       <c r="D86" s="41" t="s">
         <v>18</v>
       </c>
@@ -4675,49 +5041,49 @@
         <v>16</v>
       </c>
       <c r="G86" s="41" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H86" s="40" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A87" s="279"/>
+      <c r="A87" s="295"/>
       <c r="B87" s="115"/>
       <c r="C87" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="D87" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E87" s="17" t="s">
         <v>93</v>
-      </c>
-      <c r="D87" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E87" s="17" t="s">
-        <v>94</v>
       </c>
       <c r="F87" s="17" t="s">
         <v>16</v>
       </c>
       <c r="G87" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H87" s="202" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A88" s="280" t="s">
-        <v>168</v>
+      <c r="A88" s="296" t="s">
+        <v>167</v>
       </c>
       <c r="B88" s="219" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C88" s="87" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D88" s="88" t="s">
         <v>18</v>
       </c>
       <c r="E88" s="89" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F88" s="89" t="s">
         <v>12</v>
@@ -4728,34 +5094,34 @@
       <c r="H88" s="201"/>
     </row>
     <row r="89" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A89" s="281"/>
+      <c r="A89" s="297"/>
       <c r="B89" s="219" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C89" s="178" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D89" s="90" t="s">
         <v>18</v>
       </c>
       <c r="E89" s="91" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F89" s="91" t="s">
         <v>14</v>
       </c>
       <c r="G89" s="90" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H89" s="91"/>
     </row>
     <row r="90" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A90" s="282"/>
+      <c r="A90" s="298"/>
       <c r="B90" s="219" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C90" s="87" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D90" s="88" t="s">
         <v>18</v>
@@ -4772,20 +5138,20 @@
       <c r="H90" s="89"/>
     </row>
     <row r="91" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A91" s="335" t="s">
-        <v>174</v>
+      <c r="A91" s="351" t="s">
+        <v>173</v>
       </c>
       <c r="B91" s="218" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C91" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="D91" s="42" t="s">
+        <v>18</v>
+      </c>
+      <c r="E91" s="42" t="s">
         <v>99</v>
-      </c>
-      <c r="D91" s="42" t="s">
-        <v>18</v>
-      </c>
-      <c r="E91" s="42" t="s">
-        <v>100</v>
       </c>
       <c r="F91" s="42" t="s">
         <v>12</v>
@@ -4796,18 +5162,18 @@
       <c r="H91" s="42"/>
     </row>
     <row r="92" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A92" s="336"/>
+      <c r="A92" s="352"/>
       <c r="B92" s="182" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C92" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D92" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="E92" s="22" t="s">
         <v>103</v>
-      </c>
-      <c r="D92" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E92" s="22" t="s">
-        <v>104</v>
       </c>
       <c r="F92" s="42" t="s">
         <v>16</v>
@@ -4816,62 +5182,62 @@
         <v>36</v>
       </c>
       <c r="H92" s="232" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A93" s="337"/>
+      <c r="A93" s="353"/>
       <c r="B93" s="229" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C93" s="230" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D93" s="231" t="s">
         <v>18</v>
       </c>
       <c r="E93" s="202" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F93" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G93" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H93" s="202"/>
     </row>
     <row r="94" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A94" s="283" t="s">
+      <c r="A94" s="299" t="s">
+        <v>174</v>
+      </c>
+      <c r="B94" s="225" t="s">
         <v>175</v>
       </c>
-      <c r="B94" s="225" t="s">
-        <v>176</v>
-      </c>
       <c r="C94" s="226" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D94" s="227" t="s">
         <v>18</v>
       </c>
       <c r="E94" s="228" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F94" s="228" t="s">
         <v>14</v>
       </c>
       <c r="G94" s="227" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H94" s="228"/>
     </row>
     <row r="95" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A95" s="284"/>
+      <c r="A95" s="300"/>
       <c r="B95" s="116" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C95" s="92" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D95" s="93" t="s">
         <v>18</v>
@@ -4883,25 +5249,25 @@
         <v>14</v>
       </c>
       <c r="G95" s="93" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H95" s="94"/>
     </row>
     <row r="96" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A96" s="277" t="s">
-        <v>178</v>
+      <c r="A96" s="293" t="s">
+        <v>177</v>
       </c>
       <c r="B96" s="117" t="s">
+        <v>107</v>
+      </c>
+      <c r="C96" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="C96" s="26" t="s">
+      <c r="D96" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E96" s="45" t="s">
         <v>109</v>
-      </c>
-      <c r="D96" s="43" t="s">
-        <v>18</v>
-      </c>
-      <c r="E96" s="45" t="s">
-        <v>110</v>
       </c>
       <c r="F96" s="22" t="s">
         <v>12</v>
@@ -4912,18 +5278,18 @@
       <c r="H96" s="43"/>
     </row>
     <row r="97" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A97" s="278"/>
+      <c r="A97" s="294"/>
       <c r="B97" s="183" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C97" s="36" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D97" s="42" t="s">
         <v>18</v>
       </c>
       <c r="E97" s="42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F97" s="42" t="s">
         <v>16</v>
@@ -4932,48 +5298,48 @@
         <v>36</v>
       </c>
       <c r="H97" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A98" s="279"/>
+      <c r="A98" s="295"/>
       <c r="B98" s="233" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C98" s="26" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D98" s="22" t="s">
         <v>18</v>
       </c>
       <c r="E98" s="22" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F98" s="22" t="s">
         <v>15</v>
       </c>
       <c r="G98" s="15" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H98" s="22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A99" s="335" t="s">
-        <v>225</v>
+      <c r="A99" s="351" t="s">
+        <v>224</v>
       </c>
       <c r="B99" s="181" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C99" s="36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D99" s="37" t="s">
         <v>18</v>
       </c>
       <c r="E99" s="42" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F99" s="42" t="s">
         <v>12</v>
@@ -4984,36 +5350,36 @@
       <c r="H99" s="42"/>
     </row>
     <row r="100" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A100" s="279"/>
+      <c r="A100" s="295"/>
       <c r="B100" s="113" t="s">
+        <v>225</v>
+      </c>
+      <c r="C100" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="D100" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E100" s="17" t="s">
         <v>226</v>
       </c>
-      <c r="C100" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="D100" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E100" s="17" t="s">
-        <v>227</v>
-      </c>
       <c r="F100" s="17" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="G100" s="18" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H100" s="17"/>
     </row>
     <row r="101" spans="1:8" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A101" s="277" t="s">
-        <v>253</v>
+      <c r="A101" s="293" t="s">
+        <v>252</v>
       </c>
       <c r="B101" s="176" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C101" s="248" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D101" s="248" t="s">
         <v>18</v>
@@ -5030,42 +5396,42 @@
       <c r="H101" s="250"/>
     </row>
     <row r="102" spans="1:8" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A102" s="279"/>
+      <c r="A102" s="295"/>
       <c r="B102" s="113" t="s">
+        <v>253</v>
+      </c>
+      <c r="C102" s="20" t="s">
         <v>254</v>
       </c>
-      <c r="C102" s="20" t="s">
+      <c r="D102" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="E102" s="17" t="s">
         <v>255</v>
       </c>
-      <c r="D102" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="E102" s="17" t="s">
+      <c r="F102" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="G102" s="18" t="s">
         <v>256</v>
-      </c>
-      <c r="F102" s="17" t="s">
-        <v>231</v>
-      </c>
-      <c r="G102" s="18" t="s">
-        <v>257</v>
       </c>
       <c r="H102" s="17"/>
     </row>
     <row r="103" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A103" s="29" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B103" s="118" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C103" s="6" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D103" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E103" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>12</v>
@@ -5076,36 +5442,36 @@
       <c r="H103" s="3"/>
     </row>
     <row r="104" spans="1:8" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A104" s="277" t="s">
-        <v>182</v>
+      <c r="A104" s="293" t="s">
+        <v>181</v>
       </c>
       <c r="B104" s="176" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C104" s="248" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D104" s="249" t="s">
         <v>18</v>
       </c>
       <c r="E104" s="250" t="s">
+        <v>219</v>
+      </c>
+      <c r="F104" s="250" t="s">
+        <v>230</v>
+      </c>
+      <c r="G104" s="249" t="s">
         <v>220</v>
       </c>
-      <c r="F104" s="250" t="s">
-        <v>231</v>
-      </c>
-      <c r="G104" s="249" t="s">
-        <v>221</v>
-      </c>
       <c r="H104" s="250"/>
     </row>
     <row r="105" spans="1:8" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A105" s="279"/>
+      <c r="A105" s="295"/>
       <c r="B105" s="113" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C105" s="20" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D105" s="18" t="s">
         <v>18</v>
@@ -5123,19 +5489,19 @@
     </row>
     <row r="106" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A106" s="29" t="s">
+        <v>182</v>
+      </c>
+      <c r="B106" s="118" t="s">
         <v>183</v>
       </c>
-      <c r="B106" s="118" t="s">
-        <v>184</v>
-      </c>
       <c r="C106" s="6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D106" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E106" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>15</v>
@@ -5147,19 +5513,19 @@
     </row>
     <row r="107" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A107" s="29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B107" s="118" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C107" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D107" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E107" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>15</v>
@@ -5171,13 +5537,13 @@
     </row>
     <row r="108" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A108" s="29" t="s">
+        <v>185</v>
+      </c>
+      <c r="B108" s="118" t="s">
         <v>186</v>
       </c>
-      <c r="B108" s="118" t="s">
-        <v>187</v>
-      </c>
       <c r="C108" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D108" s="14" t="s">
         <v>18</v>
@@ -5192,24 +5558,24 @@
         <v>36</v>
       </c>
       <c r="H108" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A109" s="29" t="s">
+        <v>188</v>
+      </c>
+      <c r="B109" s="118" t="s">
         <v>189</v>
       </c>
-      <c r="B109" s="118" t="s">
-        <v>190</v>
-      </c>
       <c r="C109" s="6" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D109" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E109" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>16</v>
@@ -5218,24 +5584,24 @@
         <v>36</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A110" s="29" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B110" s="118" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C110" s="6" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D110" s="14" t="s">
         <v>18</v>
       </c>
       <c r="E110" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>16</v>
@@ -5244,50 +5610,50 @@
         <v>36</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="111" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A111" s="30" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B111" s="117" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C111" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D111" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E111" s="11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F111" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G111" s="11" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H111" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="112" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A112" s="29" t="s">
+        <v>178</v>
+      </c>
+      <c r="B112" s="119" t="s">
         <v>179</v>
       </c>
-      <c r="B112" s="119" t="s">
-        <v>180</v>
-      </c>
       <c r="C112" s="45" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D112" s="44" t="s">
         <v>18</v>
       </c>
       <c r="E112" s="43" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F112" s="43" t="s">
         <v>21</v>
@@ -5298,12 +5664,12 @@
       <c r="H112" s="43"/>
     </row>
     <row r="113" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A113" s="261" t="s">
-        <v>193</v>
+      <c r="A113" s="277" t="s">
+        <v>192</v>
       </c>
       <c r="B113" s="184"/>
-      <c r="C113" s="307" t="s">
-        <v>135</v>
+      <c r="C113" s="323" t="s">
+        <v>134</v>
       </c>
       <c r="D113" s="95" t="s">
         <v>18</v>
@@ -5318,13 +5684,13 @@
         <v>7</v>
       </c>
       <c r="H113" s="96" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="114" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A114" s="262"/>
+      <c r="A114" s="278"/>
       <c r="B114" s="184"/>
-      <c r="C114" s="308"/>
+      <c r="C114" s="324"/>
       <c r="D114" s="97" t="s">
         <v>18</v>
       </c>
@@ -5338,18 +5704,18 @@
         <v>7</v>
       </c>
       <c r="H114" s="98" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A115" s="262"/>
+      <c r="A115" s="278"/>
       <c r="B115" s="184"/>
-      <c r="C115" s="308"/>
+      <c r="C115" s="324"/>
       <c r="D115" s="100" t="s">
         <v>18</v>
       </c>
       <c r="E115" s="99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F115" s="99" t="s">
         <v>12</v>
@@ -5358,18 +5724,18 @@
         <v>22</v>
       </c>
       <c r="H115" s="99" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="116" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A116" s="262"/>
+      <c r="A116" s="278"/>
       <c r="B116" s="185"/>
-      <c r="C116" s="308"/>
+      <c r="C116" s="324"/>
       <c r="D116" s="100" t="s">
         <v>18</v>
       </c>
       <c r="E116" s="99" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F116" s="99" t="s">
         <v>14</v>
@@ -5378,40 +5744,40 @@
         <v>11</v>
       </c>
       <c r="H116" s="99" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A117" s="278"/>
+      <c r="B117" s="186"/>
+      <c r="C117" s="325"/>
+      <c r="D117" s="101" t="s">
+        <v>18</v>
+      </c>
+      <c r="E117" s="102" t="s">
         <v>138</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A117" s="262"/>
-      <c r="B117" s="186"/>
-      <c r="C117" s="309"/>
-      <c r="D117" s="101" t="s">
-        <v>18</v>
-      </c>
-      <c r="E117" s="102" t="s">
-        <v>139</v>
       </c>
       <c r="F117" s="102" t="s">
         <v>16</v>
       </c>
       <c r="G117" s="101" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H117" s="102" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="118" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
-      <c r="A118" s="262"/>
+      <c r="A118" s="278"/>
       <c r="B118" s="186"/>
-      <c r="C118" s="259" t="s">
-        <v>140</v>
+      <c r="C118" s="275" t="s">
+        <v>139</v>
       </c>
       <c r="D118" s="103" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E118" s="104" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F118" s="104" t="s">
         <v>14</v>
@@ -5420,98 +5786,98 @@
         <v>11</v>
       </c>
       <c r="H118" s="104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="119" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A119" s="262"/>
+      <c r="A119" s="278"/>
       <c r="B119" s="186"/>
-      <c r="C119" s="260"/>
+      <c r="C119" s="276"/>
       <c r="D119" s="105" t="s">
         <v>18</v>
       </c>
       <c r="E119" s="106" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F119" s="106" t="s">
         <v>16</v>
       </c>
       <c r="G119" s="105" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H119" s="106" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A120" s="263"/>
+      <c r="A120" s="279"/>
       <c r="B120" s="187"/>
       <c r="C120" s="217" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D120" s="145" t="s">
         <v>18</v>
       </c>
       <c r="E120" s="146" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F120" s="146" t="s">
         <v>16</v>
       </c>
       <c r="G120" s="147" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H120" s="107" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="121" spans="1:8" ht="18" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A121" s="328" t="s">
-        <v>201</v>
+      <c r="A121" s="344" t="s">
+        <v>200</v>
       </c>
       <c r="B121" s="150"/>
       <c r="C121" s="11" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D121" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E121" s="11" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F121" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G121" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G121" s="11" t="s">
-        <v>200</v>
-      </c>
       <c r="H121" s="19"/>
     </row>
     <row r="122" spans="1:8" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A122" s="329"/>
+      <c r="A122" s="345"/>
       <c r="B122" s="151"/>
       <c r="C122" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>18</v>
       </c>
       <c r="E122" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F122" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G122" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G122" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="H122" s="2"/>
     </row>
     <row r="123" spans="1:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A123" s="330"/>
+      <c r="A123" s="346"/>
       <c r="B123" s="153"/>
       <c r="C123" s="25" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D123" s="25" t="s">
         <v>18</v>
@@ -5520,172 +5886,172 @@
         <v>40</v>
       </c>
       <c r="F123" s="12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G123" s="25" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H123" s="25"/>
     </row>
     <row r="124" spans="1:8" ht="18.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A124" s="328" t="s">
-        <v>209</v>
+      <c r="A124" s="344" t="s">
+        <v>208</v>
       </c>
       <c r="B124" s="150"/>
       <c r="C124" s="154" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D124" s="19" t="s">
         <v>18</v>
       </c>
       <c r="E124" s="156" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F124" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G124" s="11" t="s">
         <v>199</v>
       </c>
-      <c r="G124" s="11" t="s">
-        <v>200</v>
-      </c>
       <c r="H124" s="19"/>
     </row>
     <row r="125" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A125" s="329"/>
+      <c r="A125" s="345"/>
       <c r="B125" s="151"/>
       <c r="C125" s="155" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>18</v>
       </c>
       <c r="E125" s="157" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F125" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="G125" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="G125" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="H125" s="2"/>
     </row>
     <row r="126" spans="1:8" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A126" s="330"/>
+      <c r="A126" s="346"/>
       <c r="B126" s="152"/>
       <c r="C126" s="149" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D126" s="149" t="s">
         <v>18</v>
       </c>
       <c r="E126" s="158" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F126" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="G126" s="148" t="s">
         <v>199</v>
-      </c>
-      <c r="G126" s="148" t="s">
-        <v>200</v>
       </c>
       <c r="H126" s="149"/>
     </row>
     <row r="127" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A127" s="160" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B127" s="162"/>
       <c r="C127" s="149" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D127" s="149" t="s">
         <v>18</v>
       </c>
       <c r="E127" s="158" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F127" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="G127" s="148" t="s">
         <v>199</v>
-      </c>
-      <c r="G127" s="148" t="s">
-        <v>200</v>
       </c>
       <c r="H127" s="149"/>
     </row>
     <row r="128" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A128" s="161" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B128" s="163"/>
       <c r="C128" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D128" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E128" s="18" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F128" s="148" t="s">
+        <v>198</v>
+      </c>
+      <c r="G128" s="148" t="s">
         <v>199</v>
-      </c>
-      <c r="G128" s="148" t="s">
-        <v>200</v>
       </c>
       <c r="H128" s="20"/>
     </row>
     <row r="129" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A129" s="160" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B129" s="162"/>
       <c r="C129" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D129" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E129" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F129" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G129" s="6" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="H129" s="6"/>
     </row>
     <row r="130" spans="1:8" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A130" s="305" t="s">
-        <v>243</v>
+      <c r="A130" s="321" t="s">
+        <v>242</v>
       </c>
       <c r="B130" s="251" t="s">
+        <v>267</v>
+      </c>
+      <c r="C130" s="250" t="s">
+        <v>264</v>
+      </c>
+      <c r="D130" s="248" t="s">
+        <v>18</v>
+      </c>
+      <c r="E130" s="248" t="s">
+        <v>266</v>
+      </c>
+      <c r="F130" s="248" t="s">
+        <v>230</v>
+      </c>
+      <c r="G130" s="248" t="s">
+        <v>256</v>
+      </c>
+      <c r="H130" s="248"/>
+    </row>
+    <row r="131" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A131" s="322"/>
+      <c r="B131" s="252" t="s">
         <v>268</v>
       </c>
-      <c r="C130" s="250" t="s">
+      <c r="C131" s="17" t="s">
         <v>265</v>
-      </c>
-      <c r="D130" s="248" t="s">
-        <v>18</v>
-      </c>
-      <c r="E130" s="248" t="s">
-        <v>267</v>
-      </c>
-      <c r="F130" s="248" t="s">
-        <v>231</v>
-      </c>
-      <c r="G130" s="248" t="s">
-        <v>257</v>
-      </c>
-      <c r="H130" s="248"/>
-    </row>
-    <row r="131" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A131" s="306"/>
-      <c r="B131" s="252" t="s">
-        <v>269</v>
-      </c>
-      <c r="C131" s="17" t="s">
-        <v>266</v>
       </c>
       <c r="D131" s="20" t="s">
         <v>18</v>
@@ -5694,64 +6060,64 @@
         <v>34</v>
       </c>
       <c r="F131" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G131" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H131" s="20"/>
     </row>
     <row r="132" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A132" s="159" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B132" s="163"/>
       <c r="C132" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D132" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E132" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F132" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G132" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H132" s="3"/>
     </row>
     <row r="133" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A133" s="159" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B133" s="163"/>
       <c r="C133" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D133" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E133" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F133" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G133" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H133" s="3"/>
     </row>
     <row r="134" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A134" s="159" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B134" s="163"/>
       <c r="C134" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>18</v>
@@ -5760,98 +6126,98 @@
         <v>33</v>
       </c>
       <c r="F134" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G134" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H134" s="3"/>
     </row>
     <row r="135" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A135" s="159" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B135" s="163"/>
       <c r="C135" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D135" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E135" s="3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G135" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H135" s="3"/>
     </row>
     <row r="136" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A136" s="159" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B136" s="163"/>
       <c r="C136" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D136" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E136" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F136" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G136" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H136" s="3"/>
     </row>
     <row r="137" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A137" s="159" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B137" s="163"/>
       <c r="C137" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D137" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G137" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H137" s="3"/>
     </row>
     <row r="138" spans="1:8" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A138" s="159" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B138" s="163"/>
       <c r="C138" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E138" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D138" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E138" s="3" t="s">
-        <v>263</v>
-      </c>
       <c r="F138" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G138" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H138" s="3"/>
     </row>
@@ -6852,10 +7218,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6606E4FC-447B-4C4B-8667-76C225606924}">
-  <dimension ref="A1:B77"/>
+  <dimension ref="A1:B98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="G85" sqref="G85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -6869,12 +7235,12 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A2" s="45" t="s">
-        <v>132</v>
+        <v>65</v>
       </c>
       <c r="B2" s="253" t="s">
         <v>271</v>
@@ -6882,608 +7248,976 @@
     </row>
     <row r="3" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="237" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="253" t="s">
-        <v>272</v>
+        <v>234</v>
+      </c>
+      <c r="B3" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A4" s="26" t="s">
-        <v>109</v>
-      </c>
-      <c r="B4" s="253" t="s">
-        <v>273</v>
+        <v>250</v>
+      </c>
+      <c r="B4" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="36" t="s">
-        <v>114</v>
-      </c>
-      <c r="B5" s="253" t="s">
-        <v>274</v>
+        <v>88</v>
+      </c>
+      <c r="B5" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A6" t="s">
-        <v>97</v>
-      </c>
-      <c r="B6" s="253" t="s">
-        <v>275</v>
+      <c r="A6" s="15" t="s">
+        <v>260</v>
+      </c>
+      <c r="B6" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="42" t="s">
-        <v>68</v>
-      </c>
-      <c r="B7" s="253" t="s">
-        <v>276</v>
+        <v>98</v>
+      </c>
+      <c r="B7" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A8" t="s">
-        <v>105</v>
+      <c r="A8" s="15" t="s">
+        <v>257</v>
       </c>
       <c r="B8" s="253" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="36" t="s">
-        <v>49</v>
-      </c>
-      <c r="B9" s="253" t="s">
-        <v>278</v>
+        <v>91</v>
+      </c>
+      <c r="B9" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10" s="253" t="s">
-        <v>279</v>
+      <c r="A10" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" t="s">
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="B11" s="253" t="s">
-        <v>280</v>
+      <c r="B11" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="253" t="s">
-        <v>281</v>
+      <c r="A12" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="B12" t="s">
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>211</v>
-      </c>
-      <c r="B13" s="253" t="s">
-        <v>282</v>
+      <c r="A13" s="15" t="s">
+        <v>263</v>
+      </c>
+      <c r="B13" t="s">
+        <v>337</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>213</v>
-      </c>
-      <c r="B14" s="253" t="s">
-        <v>283</v>
+      <c r="A14" s="15" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A15" s="20" t="s">
-        <v>224</v>
-      </c>
-      <c r="B15" s="253" t="s">
-        <v>284</v>
+      <c r="A15" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="B15" t="s">
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>240</v>
+        <v>370</v>
       </c>
       <c r="B16" s="253" t="s">
-        <v>285</v>
+        <v>371</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A17" s="248" t="s">
-        <v>241</v>
-      </c>
-      <c r="B17" s="253" t="s">
-        <v>286</v>
+      <c r="A17" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" t="s">
+        <v>303</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A18" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="B18" s="253" t="s">
-        <v>287</v>
+        <v>61</v>
+      </c>
+      <c r="B18" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="B19" s="254" t="s">
-        <v>288</v>
+      <c r="A19" s="248" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="269" t="s">
+        <v>367</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B20" t="s">
-        <v>289</v>
+      <c r="B20" s="254" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A21" s="3" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A22" s="3" t="s">
-        <v>45</v>
+        <v>207</v>
       </c>
       <c r="B22" t="s">
-        <v>291</v>
+        <v>321</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>292</v>
+        <v>108</v>
+      </c>
+      <c r="B23" s="253" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A24" s="3" t="s">
-        <v>32</v>
+        <v>64</v>
       </c>
       <c r="B24" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A25" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B25" t="s">
-        <v>294</v>
+      <c r="A25" s="270" t="s">
+        <v>104</v>
+      </c>
+      <c r="B25" s="253" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="3" t="s">
-        <v>84</v>
+        <v>205</v>
       </c>
       <c r="B26" t="s">
-        <v>295</v>
+        <v>319</v>
       </c>
     </row>
     <row r="27" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A27" s="3" t="s">
-        <v>37</v>
+        <v>206</v>
       </c>
       <c r="B27" t="s">
-        <v>296</v>
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A28" s="3" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A29" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B29" t="s">
-        <v>298</v>
+      <c r="A29" s="270" t="s">
+        <v>144</v>
+      </c>
+      <c r="B29" s="269" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B30" t="s">
-        <v>299</v>
+      <c r="A30" s="270" t="s">
+        <v>144</v>
+      </c>
+      <c r="B30" s="253" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B31" t="s">
-        <v>300</v>
+      <c r="A31" s="270" t="s">
+        <v>212</v>
+      </c>
+      <c r="B31" s="253" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="32" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B32" t="s">
-        <v>135</v>
+        <v>258</v>
+      </c>
+      <c r="B32" s="254" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A33" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B33" t="s">
-        <v>301</v>
+        <v>239</v>
+      </c>
+      <c r="B33" s="253" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="34" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A34" s="3" t="s">
-        <v>116</v>
+        <v>213</v>
       </c>
       <c r="B34" t="s">
-        <v>302</v>
+        <v>322</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A35" s="3" t="s">
-        <v>117</v>
+        <v>77</v>
       </c>
       <c r="B35" t="s">
-        <v>303</v>
+        <v>308</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A36" s="3" t="s">
-        <v>119</v>
+        <v>261</v>
       </c>
       <c r="B36" t="s">
-        <v>119</v>
+        <v>338</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="3" t="s">
-        <v>95</v>
+        <v>118</v>
       </c>
       <c r="B37" t="s">
-        <v>304</v>
+        <v>118</v>
       </c>
     </row>
     <row r="38" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A38" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="B38" t="s">
-        <v>305</v>
+        <v>113</v>
+      </c>
+      <c r="B38" s="253" t="s">
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A39" s="3" t="s">
-        <v>140</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>140</v>
+        <v>296</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A40" s="3" t="s">
-        <v>65</v>
+        <v>215</v>
       </c>
       <c r="B40" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A41" s="3" t="s">
-        <v>96</v>
+        <v>265</v>
       </c>
       <c r="B41" t="s">
-        <v>307</v>
+        <v>340</v>
       </c>
     </row>
     <row r="42" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A42" s="3" t="s">
-        <v>70</v>
+        <v>227</v>
       </c>
       <c r="B42" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
     </row>
     <row r="43" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A43" s="3" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
       <c r="B43" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" t="s">
-        <v>310</v>
+      <c r="A44" s="270" t="s">
+        <v>210</v>
+      </c>
+      <c r="B44" s="253" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="45" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A45" s="3" t="s">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
     </row>
     <row r="46" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A46" s="3" t="s">
-        <v>106</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>312</v>
+        <v>294</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A47" s="3" t="s">
-        <v>41</v>
+        <v>221</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>329</v>
       </c>
     </row>
     <row r="48" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="3" t="s">
-        <v>75</v>
+        <v>116</v>
       </c>
       <c r="B48" t="s">
-        <v>313</v>
+        <v>302</v>
       </c>
     </row>
     <row r="49" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A49" s="3" t="s">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="B49" t="s">
-        <v>314</v>
+        <v>289</v>
       </c>
     </row>
     <row r="50" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A50" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B50" t="s">
-        <v>315</v>
+        <v>131</v>
+      </c>
+      <c r="B50" s="253" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A51" s="3" t="s">
-        <v>112</v>
+        <v>231</v>
       </c>
       <c r="B51" t="s">
-        <v>316</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A52" s="3" t="s">
-        <v>133</v>
+        <v>235</v>
       </c>
       <c r="B52" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A53" s="3" t="s">
-        <v>202</v>
+        <v>115</v>
       </c>
       <c r="B53" t="s">
-        <v>318</v>
+        <v>301</v>
       </c>
     </row>
     <row r="54" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="3" t="s">
-        <v>203</v>
+        <v>57</v>
       </c>
       <c r="B54" t="s">
-        <v>319</v>
+        <v>291</v>
       </c>
     </row>
     <row r="55" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55" s="3" t="s">
-        <v>206</v>
+        <v>111</v>
       </c>
       <c r="B55" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
     </row>
     <row r="56" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A56" s="3" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
       <c r="B56" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="57" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A57" s="3" t="s">
-        <v>208</v>
+        <v>264</v>
       </c>
       <c r="B57" t="s">
-        <v>322</v>
+        <v>339</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="3" t="s">
-        <v>214</v>
+        <v>41</v>
       </c>
       <c r="B58" t="s">
-        <v>323</v>
+        <v>41</v>
       </c>
     </row>
     <row r="59" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A59" s="3" t="s">
-        <v>215</v>
+        <v>78</v>
       </c>
       <c r="B59" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
     </row>
     <row r="60" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A60" s="3" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B60" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="3" t="s">
-        <v>218</v>
+        <v>251</v>
       </c>
       <c r="B61" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
     </row>
     <row r="62" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="3" t="s">
-        <v>235</v>
-      </c>
-      <c r="B62" t="s">
-        <v>327</v>
+      <c r="A62" s="270" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="253" t="s">
+        <v>274</v>
       </c>
     </row>
     <row r="63" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A63" s="3" t="s">
-        <v>232</v>
+        <v>132</v>
       </c>
       <c r="B63" t="s">
-        <v>328</v>
+        <v>316</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A64" s="3" t="s">
-        <v>233</v>
-      </c>
-      <c r="B64" t="s">
-        <v>329</v>
+        <v>67</v>
+      </c>
+      <c r="B64" s="253" t="s">
+        <v>275</v>
       </c>
     </row>
     <row r="65" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="3" t="s">
-        <v>222</v>
+        <v>74</v>
       </c>
       <c r="B65" t="s">
-        <v>330</v>
+        <v>312</v>
       </c>
     </row>
     <row r="66" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A66" s="3" t="s">
-        <v>229</v>
+        <v>95</v>
       </c>
       <c r="B66" t="s">
-        <v>331</v>
+        <v>306</v>
       </c>
     </row>
     <row r="67" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="B67" t="s">
-        <v>332</v>
+      <c r="A67" s="270" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67" s="253" t="s">
+        <v>280</v>
       </c>
     </row>
     <row r="68" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A68" s="3" t="s">
-        <v>236</v>
-      </c>
-      <c r="B68" t="s">
-        <v>333</v>
+      <c r="A68" s="270" t="s">
+        <v>124</v>
+      </c>
+      <c r="B68" s="253" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="3" t="s">
-        <v>251</v>
+        <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>334</v>
+        <v>307</v>
       </c>
     </row>
     <row r="70" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A70" s="3" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B70" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="3" t="s">
-        <v>255</v>
+        <v>202</v>
       </c>
       <c r="B71" t="s">
-        <v>255</v>
+        <v>318</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A72" s="3" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="B72" t="s">
-        <v>336</v>
+        <v>254</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A73" s="3" t="s">
-        <v>260</v>
+        <v>44</v>
       </c>
       <c r="B73" t="s">
-        <v>337</v>
+        <v>290</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A74" s="3" t="s">
-        <v>264</v>
+        <v>201</v>
       </c>
       <c r="B74" t="s">
-        <v>338</v>
+        <v>317</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A75" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="B75" t="s">
-        <v>339</v>
+        <v>48</v>
+      </c>
+      <c r="B75" s="253" t="s">
+        <v>277</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A76" s="3" t="s">
-        <v>265</v>
+        <v>217</v>
       </c>
       <c r="B76" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
-      <c r="A77" s="43" t="s">
-        <v>266</v>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A77" s="3" t="s">
+        <v>66</v>
       </c>
       <c r="B77" t="s">
-        <v>341</v>
-      </c>
-    </row>
+        <v>297</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A78" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B78" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A79" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B79" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A80" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="B80" s="253" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A81" s="43" t="s">
+        <v>223</v>
+      </c>
+      <c r="B81" s="253" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A82" s="138" t="s">
+        <v>35</v>
+      </c>
+      <c r="B82" s="253" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A83" s="43" t="s">
+        <v>378</v>
+      </c>
+      <c r="B83" s="253" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="A84" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="B84" s="253" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="173" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="253" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A86" s="76" t="s">
+        <v>52</v>
+      </c>
+      <c r="B86" s="253" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A87" s="85" t="s">
+        <v>80</v>
+      </c>
+      <c r="B87" s="253" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A88" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="B88" s="253" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A89" s="20" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89" s="253" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A90" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="B90" s="253" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A91" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="B91" s="253" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A92" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="B92" s="253" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A93" s="36" t="s">
+        <v>110</v>
+      </c>
+      <c r="B93" s="253" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="217" t="s">
+        <v>141</v>
+      </c>
+      <c r="B94" s="253" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A95" s="49" t="s">
+        <v>71</v>
+      </c>
+      <c r="B95" s="253" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A96" s="42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B96" s="253" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A97" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B97" s="254" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADEA23E-E81E-4AF5-920B-9A516112A0D6}">
+  <dimension ref="A1:D16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="12.90625" style="255" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.36328125" style="255" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="44.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" s="256" t="s">
+        <v>349</v>
+      </c>
+      <c r="B1" s="256" t="s">
+        <v>372</v>
+      </c>
+      <c r="C1" s="256" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1" s="255" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="257" t="s">
+        <v>341</v>
+      </c>
+      <c r="B2" s="257" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="27"/>
+      <c r="D2" s="263"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="257" t="s">
+        <v>342</v>
+      </c>
+      <c r="B3" s="257" t="s">
+        <v>342</v>
+      </c>
+      <c r="C3" s="27"/>
+      <c r="D3" s="263"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="257" t="s">
+        <v>347</v>
+      </c>
+      <c r="B4" s="257" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="263"/>
+    </row>
+    <row r="5" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="265" t="s">
+        <v>373</v>
+      </c>
+      <c r="B5" s="265" t="s">
+        <v>350</v>
+      </c>
+      <c r="C5" s="27"/>
+      <c r="D5" s="263" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="257" t="s">
+        <v>358</v>
+      </c>
+      <c r="B6" s="257" t="s">
+        <v>358</v>
+      </c>
+      <c r="C6" s="261" t="s">
+        <v>357</v>
+      </c>
+      <c r="D6" s="263" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A7" s="257" t="s">
+        <v>376</v>
+      </c>
+      <c r="B7" s="257" t="s">
+        <v>356</v>
+      </c>
+      <c r="C7" s="260" t="s">
+        <v>351</v>
+      </c>
+      <c r="D7" s="263" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="257" t="s">
+        <v>346</v>
+      </c>
+      <c r="B8" s="257" t="s">
+        <v>346</v>
+      </c>
+      <c r="C8" s="261"/>
+      <c r="D8" s="263"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="257" t="s">
+        <v>345</v>
+      </c>
+      <c r="B9" s="257" t="s">
+        <v>345</v>
+      </c>
+      <c r="C9" s="261"/>
+      <c r="D9" s="263"/>
+    </row>
+    <row r="10" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A10" s="266" t="s">
+        <v>344</v>
+      </c>
+      <c r="B10" s="266" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" s="261"/>
+      <c r="D10" s="268" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A11" s="267" t="s">
+        <v>374</v>
+      </c>
+      <c r="B11" s="267" t="s">
+        <v>352</v>
+      </c>
+      <c r="C11" s="27"/>
+      <c r="D11" s="268" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="259" t="s">
+        <v>348</v>
+      </c>
+      <c r="B12" s="259" t="s">
+        <v>348</v>
+      </c>
+      <c r="C12" s="261"/>
+      <c r="D12" s="263"/>
+    </row>
+    <row r="13" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="257" t="s">
+        <v>343</v>
+      </c>
+      <c r="B13" s="257" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" s="260" t="s">
+        <v>343</v>
+      </c>
+      <c r="D13" s="263" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="258" t="s">
+        <v>375</v>
+      </c>
+      <c r="B14" s="258" t="s">
+        <v>355</v>
+      </c>
+      <c r="C14" s="261"/>
+      <c r="D14" s="264" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+      <c r="A15" s="258" t="s">
+        <v>361</v>
+      </c>
+      <c r="B15" s="258" t="s">
+        <v>361</v>
+      </c>
+      <c r="C15" s="262" t="s">
+        <v>362</v>
+      </c>
+      <c r="D15" s="263" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35"/>
+  </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>